<commit_message>
add 2 code cambodia 20230324
</commit_message>
<xml_diff>
--- a/uploads/(Formatted)-20230303 Clinics - VN - Latest.xlsx
+++ b/uploads/(Formatted)-20230303 Clinics - VN - Latest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michace/Desktop/SAS/tools/sas-export-clinics-from-excel/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBD6F01-02AB-444A-82D4-EE83F9D4B118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443F2924-A039-5742-851D-802F5C1897CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45700" yWindow="2740" windowWidth="34560" windowHeight="20340" xr2:uid="{CD5FCDE9-40CA-A645-8A7E-D71150EC814D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20280" xr2:uid="{CD5FCDE9-40CA-A645-8A7E-D71150EC814D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7051" uniqueCount="3375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7098" uniqueCount="3407">
   <si>
     <t>Tiếng Việt</t>
   </si>
@@ -10323,6 +10323,102 @@
   </si>
   <si>
     <t>786 Nguyen Kiem, Ward 3 Go Vap District Ho Chi Minh</t>
+  </si>
+  <si>
+    <t>KIC2004</t>
+  </si>
+  <si>
+    <t>មន្ទីរសំរ៉ាកព្យាបាលខេម៉ា2004</t>
+  </si>
+  <si>
+    <t># 036 ផ្លូវ2004 ខណ្ឌ័សែនសុខ ភ្នំពេញ, ខណ្ឌ័សែនសុខ, ភ្នំពេញ</t>
+  </si>
+  <si>
+    <t>ខណ្ឌ័សែនសុខ</t>
+  </si>
+  <si>
+    <t>25 ម៉ោង ចាប់ពីចន្ទ័ដល់់ថ្ងៃអាទិត្យ</t>
+  </si>
+  <si>
+    <t>ជំងឺទូទៅ</t>
+  </si>
+  <si>
+    <t>ភ្នំពេញ</t>
+  </si>
+  <si>
+    <t>KHEMA CLINIC STREET 2004</t>
+  </si>
+  <si>
+    <t>#036 Street 2004</t>
+  </si>
+  <si>
+    <t>Khan Sen Sok</t>
+  </si>
+  <si>
+    <t>Phnom Penh</t>
+  </si>
+  <si>
+    <t>104.88053623938677</t>
+  </si>
+  <si>
+    <t>ផ្លូវ2004 ខណ្ឌ័សែនសុខ ភ្នំពេញ, ខណ្ឌ័សែនសុខ, ភ្នំពេញ</t>
+  </si>
+  <si>
+    <t>#036 Street 2004, Khan Sen Sok , Phnom Penh</t>
+  </si>
+  <si>
+    <t>cambodia</t>
+  </si>
+  <si>
+    <t>KH</t>
+  </si>
+  <si>
+    <t>KIC</t>
+  </si>
+  <si>
+    <t>មន្ទីរសំរ៉ាកព្យាបាលខេម៉ា</t>
+  </si>
+  <si>
+    <t>ខណ្ឌ័ចំការមន</t>
+  </si>
+  <si>
+    <t>KHEMA CLINIC BKK</t>
+  </si>
+  <si>
+    <t>#28 Street 294, Boeung Keng Kang I</t>
+  </si>
+  <si>
+    <t>Khan Chamkamorn</t>
+  </si>
+  <si>
+    <t>104.9304520682222</t>
+  </si>
+  <si>
+    <t>#28 Street 294, Boeung Keng Kang I, Khan Chamkarmon, Phnom Penh</t>
+  </si>
+  <si>
+    <t>Mon– Sun: 24/7</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>11,5624780807692</t>
+  </si>
+  <si>
+    <t>(+855) 89 22 37 87</t>
+  </si>
+  <si>
+    <t>(+855) 099 222411</t>
+  </si>
+  <si>
+    <t>(+855) 099 22241</t>
+  </si>
+  <si>
+    <t>No.28, ផ្លូវ294 ផ្លូវនរត្តម, សង្កាត់ទន្លេបាសាក់ ខណ្ឌ័ចំការមន ភ្នំពេញ, ខណ្ឌ័ចំការមន, ភ្នំពេញ</t>
+  </si>
+  <si>
+    <t>No.28,  ផ្លូវ294 ផ្លូវនរត្តម, សង្កាត់ទន្លេបាសាក់ ខណ្ឌ័ចំការមន ភ្នំពេញ, ខណ្ឌ័ចំការមន, ភ្នំពេញ</t>
   </si>
 </sst>
 </file>
@@ -10551,7 +10647,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -10729,12 +10825,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -11098,30 +11216,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -11154,6 +11248,54 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -12188,20 +12330,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3996FE01-6E8E-7E4B-AF8A-2F606D870DA8}">
-  <dimension ref="A1:AE275"/>
+  <dimension ref="A1:AE277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" zoomScale="92" workbookViewId="0">
-      <selection activeCell="A272" sqref="A272:A275"/>
+    <sheetView tabSelected="1" topLeftCell="Y261" zoomScale="94" workbookViewId="0">
+      <selection activeCell="AA278" sqref="AA278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
     <col min="3" max="3" width="64.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="65.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" customWidth="1"/>
     <col min="7" max="7" width="51" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="239.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
@@ -12215,7 +12357,9 @@
     <col min="17" max="17" width="98.83203125" bestFit="1" customWidth="1"/>
     <col min="18" max="20" width="3.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="34.33203125" customWidth="1"/>
+    <col min="25" max="25" width="35.5" customWidth="1"/>
     <col min="26" max="26" width="95.33203125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="102.83203125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8.6640625" bestFit="1" customWidth="1"/>
@@ -12234,36 +12378,36 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="4"/>
-      <c r="J1" s="125" t="s">
+      <c r="J1" s="136" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
-      <c r="M1" s="125"/>
-      <c r="N1" s="125"/>
-      <c r="O1" s="125"/>
-      <c r="P1" s="125"/>
+      <c r="K1" s="136"/>
+      <c r="L1" s="136"/>
+      <c r="M1" s="136"/>
+      <c r="N1" s="136"/>
+      <c r="O1" s="136"/>
+      <c r="P1" s="136"/>
       <c r="Q1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="126" t="s">
+      <c r="R1" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="126"/>
-      <c r="T1" s="126"/>
-      <c r="U1" s="127" t="s">
+      <c r="S1" s="137"/>
+      <c r="T1" s="137"/>
+      <c r="U1" s="138" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="127"/>
-      <c r="W1" s="128" t="s">
+      <c r="V1" s="138"/>
+      <c r="W1" s="139" t="s">
         <v>5</v>
       </c>
-      <c r="X1" s="129"/>
-      <c r="Y1" s="130"/>
-      <c r="Z1" s="131" t="s">
+      <c r="X1" s="140"/>
+      <c r="Y1" s="141"/>
+      <c r="Z1" s="142" t="s">
         <v>6</v>
       </c>
-      <c r="AA1" s="132"/>
+      <c r="AA1" s="143"/>
     </row>
     <row r="2" spans="1:29" ht="154" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
@@ -34842,15 +34986,15 @@
       <c r="Q272" s="107" t="s">
         <v>3047</v>
       </c>
-      <c r="R272" s="133" t="s">
-        <v>51</v>
-      </c>
-      <c r="S272" s="133" t="s">
-        <v>51</v>
-      </c>
-      <c r="T272" s="133"/>
-      <c r="U272" s="133"/>
-      <c r="V272" s="133"/>
+      <c r="R272" s="125" t="s">
+        <v>51</v>
+      </c>
+      <c r="S272" s="125" t="s">
+        <v>51</v>
+      </c>
+      <c r="T272" s="125"/>
+      <c r="U272" s="125"/>
+      <c r="V272" s="125"/>
       <c r="W272" s="28">
         <v>10.8033940385126</v>
       </c>
@@ -34919,15 +35063,15 @@
       <c r="Q273" s="107" t="s">
         <v>3047</v>
       </c>
-      <c r="R273" s="133" t="s">
-        <v>51</v>
-      </c>
-      <c r="S273" s="133" t="s">
-        <v>51</v>
-      </c>
-      <c r="T273" s="133"/>
-      <c r="U273" s="133"/>
-      <c r="V273" s="133"/>
+      <c r="R273" s="125" t="s">
+        <v>51</v>
+      </c>
+      <c r="S273" s="125" t="s">
+        <v>51</v>
+      </c>
+      <c r="T273" s="125"/>
+      <c r="U273" s="125"/>
+      <c r="V273" s="125"/>
       <c r="W273" s="28">
         <v>10.806147372626199</v>
       </c>
@@ -34952,59 +35096,59 @@
       <c r="A274" s="118" t="s">
         <v>3354</v>
       </c>
-      <c r="B274" s="134" t="s">
+      <c r="B274" s="126" t="s">
         <v>1070</v>
       </c>
       <c r="C274" s="80" t="s">
         <v>3355</v>
       </c>
-      <c r="D274" s="135" t="s">
+      <c r="D274" s="127" t="s">
         <v>3356</v>
       </c>
-      <c r="E274" s="136" t="s">
+      <c r="E274" s="128" t="s">
         <v>214</v>
       </c>
-      <c r="F274" s="137">
+      <c r="F274" s="129">
         <v>1900636893</v>
       </c>
-      <c r="G274" s="138" t="s">
+      <c r="G274" s="130" t="s">
         <v>3341</v>
       </c>
       <c r="H274" s="96"/>
-      <c r="I274" s="139" t="s">
+      <c r="I274" s="131" t="s">
         <v>63</v>
       </c>
       <c r="J274" s="83" t="s">
         <v>3357</v>
       </c>
-      <c r="K274" s="138" t="s">
+      <c r="K274" s="130" t="s">
         <v>3358</v>
       </c>
-      <c r="L274" s="140" t="s">
+      <c r="L274" s="132" t="s">
         <v>219</v>
       </c>
-      <c r="M274" s="141">
+      <c r="M274" s="133">
         <v>1900636893</v>
       </c>
-      <c r="N274" s="138" t="s">
+      <c r="N274" s="130" t="s">
         <v>3344</v>
       </c>
-      <c r="O274" s="142"/>
-      <c r="P274" s="139" t="s">
+      <c r="O274" s="134"/>
+      <c r="P274" s="131" t="s">
         <v>69</v>
       </c>
-      <c r="Q274" s="143" t="s">
+      <c r="Q274" s="135" t="s">
         <v>3047</v>
       </c>
-      <c r="R274" s="133" t="s">
-        <v>51</v>
-      </c>
-      <c r="S274" s="133" t="s">
-        <v>51</v>
-      </c>
-      <c r="T274" s="133"/>
-      <c r="U274" s="133"/>
-      <c r="V274" s="133"/>
+      <c r="R274" s="125" t="s">
+        <v>51</v>
+      </c>
+      <c r="S274" s="125" t="s">
+        <v>51</v>
+      </c>
+      <c r="T274" s="125"/>
+      <c r="U274" s="125"/>
+      <c r="V274" s="125"/>
       <c r="W274" s="28">
         <v>21.031300230512599</v>
       </c>
@@ -35032,65 +35176,65 @@
       <c r="A275" s="118" t="s">
         <v>3362</v>
       </c>
-      <c r="B275" s="134" t="s">
+      <c r="B275" s="126" t="s">
         <v>37</v>
       </c>
       <c r="C275" s="80" t="s">
         <v>3363</v>
       </c>
-      <c r="D275" s="135" t="s">
+      <c r="D275" s="127" t="s">
         <v>3364</v>
       </c>
-      <c r="E275" s="136" t="s">
+      <c r="E275" s="128" t="s">
         <v>228</v>
       </c>
-      <c r="F275" s="137" t="s">
+      <c r="F275" s="129" t="s">
         <v>3365</v>
       </c>
-      <c r="G275" s="138" t="s">
+      <c r="G275" s="130" t="s">
         <v>3366</v>
       </c>
       <c r="H275" s="96" t="s">
         <v>3367</v>
       </c>
-      <c r="I275" s="139" t="s">
+      <c r="I275" s="131" t="s">
         <v>43</v>
       </c>
       <c r="J275" s="83" t="s">
         <v>3368</v>
       </c>
-      <c r="K275" s="138" t="s">
+      <c r="K275" s="130" t="s">
         <v>3369</v>
       </c>
-      <c r="L275" s="140" t="s">
+      <c r="L275" s="132" t="s">
         <v>233</v>
       </c>
-      <c r="M275" s="141" t="s">
+      <c r="M275" s="133" t="s">
         <v>3365</v>
       </c>
-      <c r="N275" s="138" t="s">
+      <c r="N275" s="130" t="s">
         <v>3370</v>
       </c>
-      <c r="O275" s="142" t="s">
+      <c r="O275" s="134" t="s">
         <v>3371</v>
       </c>
-      <c r="P275" s="139" t="s">
+      <c r="P275" s="131" t="s">
         <v>49</v>
       </c>
-      <c r="Q275" s="143" t="s">
+      <c r="Q275" s="135" t="s">
         <v>3372</v>
       </c>
-      <c r="R275" s="133"/>
-      <c r="S275" s="133" t="s">
-        <v>51</v>
-      </c>
-      <c r="T275" s="133" t="s">
-        <v>51</v>
-      </c>
-      <c r="U275" s="133" t="s">
-        <v>51</v>
-      </c>
-      <c r="V275" s="133"/>
+      <c r="R275" s="125"/>
+      <c r="S275" s="125" t="s">
+        <v>51</v>
+      </c>
+      <c r="T275" s="125" t="s">
+        <v>51</v>
+      </c>
+      <c r="U275" s="125" t="s">
+        <v>51</v>
+      </c>
+      <c r="V275" s="125"/>
       <c r="W275" s="28">
         <v>10.820034856568199</v>
       </c>
@@ -35109,6 +35253,166 @@
       </c>
       <c r="AC275" s="115" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="276" spans="1:31" ht="17" x14ac:dyDescent="0.2">
+      <c r="A276" s="30" t="s">
+        <v>3375</v>
+      </c>
+      <c r="B276" s="126" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C276" s="151" t="s">
+        <v>3376</v>
+      </c>
+      <c r="D276" s="86" t="s">
+        <v>3377</v>
+      </c>
+      <c r="E276" s="61" t="s">
+        <v>3378</v>
+      </c>
+      <c r="F276" s="34" t="s">
+        <v>3403</v>
+      </c>
+      <c r="G276" s="34" t="s">
+        <v>3379</v>
+      </c>
+      <c r="H276" s="30" t="s">
+        <v>3380</v>
+      </c>
+      <c r="I276" s="61" t="s">
+        <v>3381</v>
+      </c>
+      <c r="J276" s="144" t="s">
+        <v>3382</v>
+      </c>
+      <c r="K276" s="86" t="s">
+        <v>3383</v>
+      </c>
+      <c r="L276" s="24" t="s">
+        <v>3384</v>
+      </c>
+      <c r="M276" s="144" t="s">
+        <v>3404</v>
+      </c>
+      <c r="N276" s="130" t="s">
+        <v>3399</v>
+      </c>
+      <c r="O276" s="23" t="s">
+        <v>3400</v>
+      </c>
+      <c r="P276" s="24" t="s">
+        <v>3385</v>
+      </c>
+      <c r="Q276" s="145"/>
+      <c r="R276" s="26"/>
+      <c r="S276" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="T276" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="U276" s="30"/>
+      <c r="V276" s="30"/>
+      <c r="W276" s="150" t="s">
+        <v>3401</v>
+      </c>
+      <c r="X276" s="147" t="s">
+        <v>3386</v>
+      </c>
+      <c r="Y276" s="148"/>
+      <c r="Z276" s="149" t="s">
+        <v>3387</v>
+      </c>
+      <c r="AA276" s="149" t="s">
+        <v>3388</v>
+      </c>
+      <c r="AB276" t="s">
+        <v>3389</v>
+      </c>
+      <c r="AC276" t="s">
+        <v>3390</v>
+      </c>
+    </row>
+    <row r="277" spans="1:31" ht="28" x14ac:dyDescent="0.2">
+      <c r="A277" s="30" t="s">
+        <v>3391</v>
+      </c>
+      <c r="B277" s="126" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C277" s="151" t="s">
+        <v>3392</v>
+      </c>
+      <c r="D277" s="86" t="s">
+        <v>3405</v>
+      </c>
+      <c r="E277" s="61" t="s">
+        <v>3393</v>
+      </c>
+      <c r="F277" s="34" t="s">
+        <v>3402</v>
+      </c>
+      <c r="G277" s="34" t="s">
+        <v>3379</v>
+      </c>
+      <c r="H277" s="30" t="s">
+        <v>3380</v>
+      </c>
+      <c r="I277" s="61" t="s">
+        <v>3381</v>
+      </c>
+      <c r="J277" s="144" t="s">
+        <v>3394</v>
+      </c>
+      <c r="K277" s="86" t="s">
+        <v>3395</v>
+      </c>
+      <c r="L277" s="24" t="s">
+        <v>3396</v>
+      </c>
+      <c r="M277" s="144" t="s">
+        <v>3402</v>
+      </c>
+      <c r="N277" s="130" t="s">
+        <v>3399</v>
+      </c>
+      <c r="O277" s="23" t="s">
+        <v>3400</v>
+      </c>
+      <c r="P277" s="24" t="s">
+        <v>3385</v>
+      </c>
+      <c r="Q277" s="145"/>
+      <c r="R277" s="26"/>
+      <c r="S277" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="T277" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="U277" s="30"/>
+      <c r="V277" s="30"/>
+      <c r="W277" s="146">
+        <v>11.5311173745487</v>
+      </c>
+      <c r="X277" s="147" t="s">
+        <v>3397</v>
+      </c>
+      <c r="Y277" s="148">
+        <v>12354</v>
+      </c>
+      <c r="Z277" s="149" t="s">
+        <v>3406</v>
+      </c>
+      <c r="AA277" s="149" t="s">
+        <v>3398</v>
+      </c>
+      <c r="AB277" t="s">
+        <v>3389</v>
+      </c>
+      <c r="AC277" t="s">
+        <v>3390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>